<commit_message>
Compilata colonna J della checklist per testcase 47 e 48
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111#SNBSRLXX/SNB/WebMed/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111#SNBSRLXX/SNB/WebMed/1.0.0/report-checklist.xlsx
@@ -2861,11 +2861,11 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="T10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
-      <selection pane="bottomRight" activeCell="H53" activeCellId="0" sqref="H53"/>
+      <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="W14" activeCellId="0" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3417,7 +3417,7 @@
       <c r="H14" s="31"/>
       <c r="I14" s="32"/>
       <c r="J14" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K14" s="33" t="s">
         <v>72</v>
@@ -3474,7 +3474,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="32"/>
       <c r="J15" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K15" s="33" t="s">
         <v>72</v>

</xml_diff>